<commit_message>
updating to reflect 2020 standards approved by USATF on 5/20/20
</commit_message>
<xml_diff>
--- a/data/Age_Grading_Boston_Qualifying_Times.xlsx
+++ b/data/Age_Grading_Boston_Qualifying_Times.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erinm\Documents\nss-capstone\Too_Large\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erinm\Documents\nss-capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7946B4B-3940-485E-8468-26B11F604FBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B125C2-1C65-411B-A604-C7F7D605FD00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{A0544397-134C-4C61-AE87-6E75F9DBCE4D}"/>
   </bookViews>
@@ -734,6 +734,15 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -773,15 +782,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,20 +789,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="76">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2998,6 +2984,20 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3046,7 +3046,13 @@
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="4">
+        <row r="2">
+          <cell r="B2">
+            <v>18</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
@@ -3065,7 +3071,13 @@
       </sheetData>
       <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
+      <sheetData sheetId="11">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Sex</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="12"/>
       <sheetData sheetId="13">
         <row r="1">
@@ -3094,27 +3106,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="bos_17"/>
-      <sheetName val="2020_Road Weights"/>
-      <sheetName val="ORIGINAL CSV (Boston 2017)"/>
-      <sheetName val="ORIGINAL source information"/>
-      <sheetName val="boston_marathon_results_2017"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="2020_Road Weights"/>
       <sheetName val="bos_18"/>
       <sheetName val="ORIGINAL CSV (Boston 2018)"/>
@@ -3132,7 +3123,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3153,6 +3144,25 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="2020_Road Weights"/>
+      <sheetName val="bos_10"/>
+      <sheetName val="ORIGINAL CSV (Boston 2010)"/>
+      <sheetName val="ORIGINAL source information"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -3163,10 +3173,10 @@
       <sheetName val="ORIGINAL source information"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3201,16 +3211,16 @@
       <sheetName val="BQs_over_time"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9">
         <row r="4">
           <cell r="B4">
             <v>22853</v>
@@ -3223,19 +3233,25 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22">
+        <row r="1">
+          <cell r="P1">
+            <v>1.1458333333333333E-3</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3265,26 +3281,20 @@
       <sheetName val="bos_19_AG"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Sex</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
       <sheetData sheetId="14">
         <row r="12">
           <cell r="L12">
@@ -3303,36 +3313,15 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="2020_Road Weights"/>
-      <sheetName val="bos_10"/>
-      <sheetName val="ORIGINAL CSV (Boston 2010)"/>
-      <sheetName val="ORIGINAL source information"/>
-      <sheetName val="boston_marathon_results_2010"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3353,7 +3342,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3374,7 +3363,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3395,7 +3384,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3416,7 +3405,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3437,175 +3426,196 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="bos_17"/>
+      <sheetName val="2020_Road Weights"/>
+      <sheetName val="ORIGINAL CSV (Boston 2017)"/>
+      <sheetName val="ORIGINAL source information"/>
+      <sheetName val="boston_marathon_results_2017"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0C2B30FD-69C3-4A92-869F-157F76A4A88A}" name="Table2" displayName="Table2" ref="A3:F24" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74" headerRowCellStyle="Percent" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0C2B30FD-69C3-4A92-869F-157F76A4A88A}" name="Table2" displayName="Table2" ref="A3:F24" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72" headerRowCellStyle="Percent" dataCellStyle="Percent">
   <autoFilter ref="A3:F24" xr:uid="{37C56BC9-5578-43BF-A8D2-BA11A0325091}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6BED7F97-A402-4C6A-8FC9-B6997D937BAC}" name="Age" dataDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{F621C132-2210-426E-9DFD-957BDD151CBA}" name="Men (Erin)" dataDxfId="72" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{3BAD127C-83A5-4E99-ACAD-C27DC3DEC043}" name="Men (Alan)" dataDxfId="71" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{B24F780B-5B12-45B1-B7B7-2FB7364B54D5}" name="Women (Erin)" dataDxfId="70" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{4A1ED1F6-B8F3-4AC5-AC0D-DD3A61547C07}" name="Women (Alan)" dataDxfId="69" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{CD62A715-9105-4637-BD92-22E70403958F}" name="Notes re: discrepancy" dataDxfId="68" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{6BED7F97-A402-4C6A-8FC9-B6997D937BAC}" name="Age" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{F621C132-2210-426E-9DFD-957BDD151CBA}" name="Men (Erin)" dataDxfId="70" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{3BAD127C-83A5-4E99-ACAD-C27DC3DEC043}" name="Men (Alan)" dataDxfId="69" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{B24F780B-5B12-45B1-B7B7-2FB7364B54D5}" name="Women (Erin)" dataDxfId="68" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{4A1ED1F6-B8F3-4AC5-AC0D-DD3A61547C07}" name="Women (Alan)" dataDxfId="67" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{CD62A715-9105-4637-BD92-22E70403958F}" name="Notes re: discrepancy" dataDxfId="66" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BA423E9-BFC6-4DA8-BD92-47930D14153D}" name="Table1419" displayName="Table1419" ref="A5:BF72" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BA423E9-BFC6-4DA8-BD92-47930D14153D}" name="Table1419" displayName="Table1419" ref="A5:BF72" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
   <autoFilter ref="A5:BF72" xr:uid="{3DFC9418-0F22-46B2-800D-FA3A4694673A}"/>
   <tableColumns count="58">
-    <tableColumn id="2" xr3:uid="{9D658FD6-371F-48D0-A890-C9E73A7BD8F9}" name="Age" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{4FF0F157-EA33-4635-AE3E-03400083B9FA}" name="Open_Standard_Men_20" dataDxfId="63">
+    <tableColumn id="2" xr3:uid="{9D658FD6-371F-48D0-A890-C9E73A7BD8F9}" name="Age" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{4FF0F157-EA33-4635-AE3E-03400083B9FA}" name="Open_Standard_Men_20" dataDxfId="61">
       <calculatedColumnFormula>IF(BQs_over_time_AG20!$A6="","",SUMIF('2020_Road Weights'!$A:$A,"M",'2020_Road Weights'!$F:$F)/3600/24)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C78ECC2E-C27D-4745-94FF-586EED4A691A}" name="Age_Factor_Men_20" dataDxfId="62">
+    <tableColumn id="4" xr3:uid="{C78ECC2E-C27D-4745-94FF-586EED4A691A}" name="Age_Factor_Men_20" dataDxfId="60">
       <calculatedColumnFormula>IF(A6="","",INDEX('2020_Road Weights'!$A:$CX,MATCH("M",'2020_Road Weights'!$A:$A,FALSE),MATCH(BQs_over_time_AG20!$A6,'2020_Road Weights'!$1:$1,FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A6964369-114B-4E87-97C6-50C7B90F5DD1}" name="Age Best_Men_20" dataDxfId="61">
+    <tableColumn id="5" xr3:uid="{A6964369-114B-4E87-97C6-50C7B90F5DD1}" name="Age Best_Men_20" dataDxfId="59">
       <calculatedColumnFormula>IFERROR(BQs_over_time_AG20!$B6/BQs_over_time_AG20!$C6,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{614C7749-3F49-4B91-8462-1932B57A73A2}" name="QT_Men_03_12" dataDxfId="60"/>
-    <tableColumn id="13" xr3:uid="{4978BEF8-14AF-453B-9602-90B8605722D6}" name="QT_Men_03_12_min" dataDxfId="59">
+    <tableColumn id="6" xr3:uid="{614C7749-3F49-4B91-8462-1932B57A73A2}" name="QT_Men_03_12" dataDxfId="58"/>
+    <tableColumn id="13" xr3:uid="{4978BEF8-14AF-453B-9602-90B8605722D6}" name="QT_Men_03_12_min" dataDxfId="57">
       <calculatedColumnFormula>Table1419[[#This Row],[QT_Men_03_12]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EF80B7D3-F853-4198-BDAE-2466313CA6D6}" name="AG%_Men_03_12" dataDxfId="58">
+    <tableColumn id="7" xr3:uid="{EF80B7D3-F853-4198-BDAE-2466313CA6D6}" name="AG%_Men_03_12" dataDxfId="56">
       <calculatedColumnFormula>IFERROR(BQs_over_time_AG20!$D6/BQs_over_time_AG20!$E6,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FF0F9F14-9BB3-4183-9B27-2599DCF5097D}" name="AG_Time_Men_03_12" dataDxfId="57">
+    <tableColumn id="8" xr3:uid="{FF0F9F14-9BB3-4183-9B27-2599DCF5097D}" name="AG_Time_Men_03_12" dataDxfId="55">
       <calculatedColumnFormula>IFERROR(Table1419[[#This Row],[QT_Men_03_12]]*Table1419[[#This Row],[Age_Factor_Men_20]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{AEC5F439-E438-4D8B-972E-BA06B73D2017}" name="AG_Time_Men_03_12_min" dataDxfId="56">
+    <tableColumn id="15" xr3:uid="{AEC5F439-E438-4D8B-972E-BA06B73D2017}" name="AG_Time_Men_03_12_min" dataDxfId="54">
       <calculatedColumnFormula>Table1419[[#This Row],[AG_Time_Men_03_12]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A9AA2EB7-10D6-4AC9-8F38-8EDA0E86DDF9}" name="QT_Men_13_19" dataDxfId="55"/>
-    <tableColumn id="17" xr3:uid="{A202A617-0837-45CC-81F7-20302F93D1B8}" name="QT_Men_13_19_min" dataDxfId="54">
+    <tableColumn id="9" xr3:uid="{A9AA2EB7-10D6-4AC9-8F38-8EDA0E86DDF9}" name="QT_Men_13_19" dataDxfId="53"/>
+    <tableColumn id="17" xr3:uid="{A202A617-0837-45CC-81F7-20302F93D1B8}" name="QT_Men_13_19_min" dataDxfId="52">
       <calculatedColumnFormula>Table1419[[#This Row],[QT_Men_13_19]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{85FB3D6D-CA7F-421A-A550-239BDC839C66}" name="AG%_Men_13_19" dataDxfId="53">
+    <tableColumn id="10" xr3:uid="{85FB3D6D-CA7F-421A-A550-239BDC839C66}" name="AG%_Men_13_19" dataDxfId="51">
       <calculatedColumnFormula>IFERROR(BQs_over_time_AG20!$D6/BQs_over_time_AG20!$J6,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{833AF933-0A11-4DF0-9824-419AEF765224}" name="AG_Time_Men_13_19" dataDxfId="52">
+    <tableColumn id="11" xr3:uid="{833AF933-0A11-4DF0-9824-419AEF765224}" name="AG_Time_Men_13_19" dataDxfId="50">
       <calculatedColumnFormula>Table1419[[#This Row],[QT_Men_13_19]]*Table1419[[#This Row],[Age_Factor_Men_20]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{5FF94125-2C67-45A2-9E03-1F1BE76AB234}" name="AG_Time_Men_13_19_min" dataDxfId="51">
+    <tableColumn id="35" xr3:uid="{5FF94125-2C67-45A2-9E03-1F1BE76AB234}" name="AG_Time_Men_13_19_min" dataDxfId="49">
       <calculatedColumnFormula>Table1419[[#This Row],[AG_Time_Men_13_19]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{9918530F-B17B-49D8-91C3-BE635C68063B}" name="QT_Men_2020" dataDxfId="50"/>
-    <tableColumn id="36" xr3:uid="{F156E814-72F5-4D30-853B-BE2851A1C2FC}" name="QT_Men_2020_min" dataDxfId="49">
+    <tableColumn id="12" xr3:uid="{9918530F-B17B-49D8-91C3-BE635C68063B}" name="QT_Men_2020" dataDxfId="48"/>
+    <tableColumn id="36" xr3:uid="{F156E814-72F5-4D30-853B-BE2851A1C2FC}" name="QT_Men_2020_min" dataDxfId="47">
       <calculatedColumnFormula>Table1419[[#This Row],[QT_Men_2020]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{0BD0B544-C050-4923-ABAC-C28BC576AA34}" name="AG%_Men_2020" dataDxfId="48">
+    <tableColumn id="14" xr3:uid="{0BD0B544-C050-4923-ABAC-C28BC576AA34}" name="AG%_Men_2020" dataDxfId="46">
       <calculatedColumnFormula>IFERROR(BQs_over_time_AG20!$D6/BQs_over_time_AG20!$O6,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9BDE9F33-8A92-451E-AB96-A4816840CE47}" name="AG_Time_Men_2020" dataDxfId="47">
+    <tableColumn id="16" xr3:uid="{9BDE9F33-8A92-451E-AB96-A4816840CE47}" name="AG_Time_Men_2020" dataDxfId="45">
       <calculatedColumnFormula>Table1419[[#This Row],[QT_Men_2020]]*Table1419[[#This Row],[Age_Factor_Men_20]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{FD2D9976-936F-469D-B3BB-5EA30CFE3B52}" name="AG_Time_Men_2021" dataDxfId="46">
+    <tableColumn id="37" xr3:uid="{FD2D9976-936F-469D-B3BB-5EA30CFE3B52}" name="AG_Time_Men_2021" dataDxfId="44">
       <calculatedColumnFormula>Table1419[[#This Row],[AG_Time_Men_2020]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{8BB3BDA4-2A2D-4F08-B359-A320C58EFF65}" name="Open_Standard_Women" dataDxfId="45">
+    <tableColumn id="18" xr3:uid="{8BB3BDA4-2A2D-4F08-B359-A320C58EFF65}" name="Open_Standard_Women" dataDxfId="43">
       <calculatedColumnFormula>IF(BQs_over_time_AG20!$A6="","",SUMIF('2020_Road Weights'!$A:$A,"F",'2020_Road Weights'!$F:$F)/3600/24)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{AACBA22E-8F52-4833-9362-44BE0D5AAD8E}" name="Age_Factor_Women" dataDxfId="44">
+    <tableColumn id="19" xr3:uid="{AACBA22E-8F52-4833-9362-44BE0D5AAD8E}" name="Age_Factor_Women" dataDxfId="42">
       <calculatedColumnFormula>INDEX('2020_Road Weights'!$A:$CX,MATCH("F",'2020_Road Weights'!$A:$A,FALSE),MATCH(BQs_over_time_AG20!$A6,'2020_Road Weights'!$1:$1,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{2F46533F-B922-4E84-BD57-CF8A2C0D5BC2}" name="Age Best_Women" dataDxfId="43">
+    <tableColumn id="20" xr3:uid="{2F46533F-B922-4E84-BD57-CF8A2C0D5BC2}" name="Age Best_Women" dataDxfId="41">
       <calculatedColumnFormula>IFERROR(BQs_over_time_AG20!$T6/BQs_over_time_AG20!$U6,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{6DCEF499-7353-497B-B560-FE583E123CC6}" name="Qualifying_Time_Women_03_12" dataDxfId="42"/>
-    <tableColumn id="38" xr3:uid="{51748013-FBAD-452E-8593-F0AB4667790D}" name="Qualifying_Time_Women_03_12_min" dataDxfId="41">
+    <tableColumn id="21" xr3:uid="{6DCEF499-7353-497B-B560-FE583E123CC6}" name="Qualifying_Time_Women_03_12" dataDxfId="40"/>
+    <tableColumn id="38" xr3:uid="{51748013-FBAD-452E-8593-F0AB4667790D}" name="Qualifying_Time_Women_03_12_min" dataDxfId="39">
       <calculatedColumnFormula>Table1419[[#This Row],[Qualifying_Time_Women_03_12]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{3BE761D5-3BD4-43A1-B8D4-E100612067A2}" name="AG%_Women_03_12" dataDxfId="40">
+    <tableColumn id="22" xr3:uid="{3BE761D5-3BD4-43A1-B8D4-E100612067A2}" name="AG%_Women_03_12" dataDxfId="38">
       <calculatedColumnFormula>IFERROR(BQs_over_time_AG20!$V6/BQs_over_time_AG20!$W6,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{3B276C9A-8DC9-4344-A9B4-28A3E614F95C}" name="AG_Time_Women_03_12" dataDxfId="39">
+    <tableColumn id="23" xr3:uid="{3B276C9A-8DC9-4344-A9B4-28A3E614F95C}" name="AG_Time_Women_03_12" dataDxfId="37">
       <calculatedColumnFormula>Table1419[[#This Row],[Qualifying_Time_Women_03_12]]*Table1419[[#This Row],[Age_Factor_Women]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{A69C737A-B187-4CB1-A44A-1E8248B4A67B}" name="AG_Time_Women_03_12_min" dataDxfId="38">
+    <tableColumn id="39" xr3:uid="{A69C737A-B187-4CB1-A44A-1E8248B4A67B}" name="AG_Time_Women_03_12_min" dataDxfId="36">
       <calculatedColumnFormula>Table1419[[#This Row],[AG_Time_Women_03_12]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{E3EEE647-6118-48D4-BF6C-431429464363}" name="Qualifying_Time_Women_13_19" dataDxfId="37"/>
-    <tableColumn id="40" xr3:uid="{6EA6A520-895A-492B-AD4B-B9E82054E780}" name="Qualifying_Time_Women_13_19_min" dataDxfId="36">
+    <tableColumn id="24" xr3:uid="{E3EEE647-6118-48D4-BF6C-431429464363}" name="Qualifying_Time_Women_13_19" dataDxfId="35"/>
+    <tableColumn id="40" xr3:uid="{6EA6A520-895A-492B-AD4B-B9E82054E780}" name="Qualifying_Time_Women_13_19_min" dataDxfId="34">
       <calculatedColumnFormula>Table1419[[#This Row],[Qualifying_Time_Women_13_19]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{7B8088FE-239D-49DA-B1E8-1430D8649268}" name="AG%_Women_13_19" dataDxfId="35" dataCellStyle="Percent">
+    <tableColumn id="25" xr3:uid="{7B8088FE-239D-49DA-B1E8-1430D8649268}" name="AG%_Women_13_19" dataDxfId="33" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(BQs_over_time_AG20!$V6/BQs_over_time_AG20!$AB6,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{8D7AC36A-C24E-4AC1-8C17-A82E6B3632E6}" name="AG_Time_Women_13_19" dataDxfId="34">
+    <tableColumn id="26" xr3:uid="{8D7AC36A-C24E-4AC1-8C17-A82E6B3632E6}" name="AG_Time_Women_13_19" dataDxfId="32">
       <calculatedColumnFormula>Table1419[[#This Row],[Qualifying_Time_Women_13_19]]*Table1419[[#This Row],[Age_Factor_Women]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{4D2888E6-99E6-4121-B389-D3102E84EF45}" name="AG_Time_Women_13_19_min" dataDxfId="33">
+    <tableColumn id="41" xr3:uid="{4D2888E6-99E6-4121-B389-D3102E84EF45}" name="AG_Time_Women_13_19_min" dataDxfId="31">
       <calculatedColumnFormula>Table1419[[#This Row],[AG_Time_Women_13_19]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{CD0ECD2A-4BF5-4BF5-B5D8-83984499066A}" name="Qualifying_Time_Women_2020" dataDxfId="32"/>
-    <tableColumn id="42" xr3:uid="{26B8FCBD-3B3C-4A4F-BFE6-D3DFD61F6D4E}" name="Qualifying_Time_Women_2020_min" dataDxfId="31">
+    <tableColumn id="27" xr3:uid="{CD0ECD2A-4BF5-4BF5-B5D8-83984499066A}" name="Qualifying_Time_Women_2020" dataDxfId="30"/>
+    <tableColumn id="42" xr3:uid="{26B8FCBD-3B3C-4A4F-BFE6-D3DFD61F6D4E}" name="Qualifying_Time_Women_2020_min" dataDxfId="29">
       <calculatedColumnFormula>Table1419[[#This Row],[Qualifying_Time_Women_2020]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{542CA6A5-1D47-4CED-8738-AE3E5215EB5B}" name="AG%_Women_2020" dataDxfId="30" dataCellStyle="Percent">
+    <tableColumn id="28" xr3:uid="{542CA6A5-1D47-4CED-8738-AE3E5215EB5B}" name="AG%_Women_2020" dataDxfId="28" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(BQs_over_time_AG20!$V6/BQs_over_time_AG20!$AG6,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{6924694E-A0D2-450F-BC81-98924FFA88AA}" name="AG_Time_Women_2020" dataDxfId="29">
+    <tableColumn id="29" xr3:uid="{6924694E-A0D2-450F-BC81-98924FFA88AA}" name="AG_Time_Women_2020" dataDxfId="27">
       <calculatedColumnFormula>Table1419[[#This Row],[Qualifying_Time_Women_2020]]*Table1419[[#This Row],[Age_Factor_Women]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{AAA835A0-927D-4FB9-AFC1-AA9891BC36CA}" name="AG_Time_Women_2020_min" dataDxfId="28">
+    <tableColumn id="43" xr3:uid="{AAA835A0-927D-4FB9-AFC1-AA9891BC36CA}" name="AG_Time_Women_2020_min" dataDxfId="26">
       <calculatedColumnFormula>Table1419[[#This Row],[AG_Time_Women_2020]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{3CFB6E9B-F96E-48AA-AED4-011B1DBB8B8F}" name="No Ranking" dataDxfId="27">
+    <tableColumn id="30" xr3:uid="{3CFB6E9B-F96E-48AA-AED4-011B1DBB8B8F}" name="No Ranking" dataDxfId="25">
       <calculatedColumnFormula>$AL$4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{016F76B8-D570-4FC9-895C-4D009A5CFA01}" name="Local Class" dataDxfId="26">
+    <tableColumn id="31" xr3:uid="{016F76B8-D570-4FC9-895C-4D009A5CFA01}" name="Local Class" dataDxfId="24">
       <calculatedColumnFormula>$AM$4-$AL$4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{B484D1EE-A3CB-4F38-9C11-B985672FC115}" name="Regional Class" dataDxfId="25">
+    <tableColumn id="32" xr3:uid="{B484D1EE-A3CB-4F38-9C11-B985672FC115}" name="Regional Class" dataDxfId="23">
       <calculatedColumnFormula>$AN$4-$AM$4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{C735F3B3-577F-44D2-AA08-B1BFED06E2DE}" name="National Class" dataDxfId="24">
+    <tableColumn id="33" xr3:uid="{C735F3B3-577F-44D2-AA08-B1BFED06E2DE}" name="National Class" dataDxfId="22">
       <calculatedColumnFormula>$AO$4-$AN$4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{48C48A9B-EF64-41AF-ACC1-57234EABB261}" name="World Class" dataDxfId="23">
+    <tableColumn id="34" xr3:uid="{48C48A9B-EF64-41AF-ACC1-57234EABB261}" name="World Class" dataDxfId="21">
       <calculatedColumnFormula>$AP$4-$AO$4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="49" xr3:uid="{2A4AF9FB-A15C-4251-94EE-696C83B7365E}" name="Proposed_uniform_AG%" dataDxfId="22"/>
-    <tableColumn id="44" xr3:uid="{0C4B66E7-8FC2-4B97-ABFD-FC7621BCFC87}" name="Proposed_QT_M" dataDxfId="21">
+    <tableColumn id="49" xr3:uid="{2A4AF9FB-A15C-4251-94EE-696C83B7365E}" name="Proposed_uniform_AG%" dataDxfId="20"/>
+    <tableColumn id="44" xr3:uid="{0C4B66E7-8FC2-4B97-ABFD-FC7621BCFC87}" name="Proposed_QT_M" dataDxfId="19">
       <calculatedColumnFormula>Table1419[[#This Row],[Age Best_Men_20]]/Table1419[[#This Row],[Proposed_uniform_AG%]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="58" xr3:uid="{03AEB66D-572A-4D3B-9E36-CDD1A39F0061}" name="Proposed_QT_M_Agegrouped" dataDxfId="20"/>
-    <tableColumn id="51" xr3:uid="{4DA2C733-ABC7-49F3-87B2-5B3B3C0229C3}" name="Proposed_QT_M_Agegrouped_roundedup" dataDxfId="19">
+    <tableColumn id="58" xr3:uid="{03AEB66D-572A-4D3B-9E36-CDD1A39F0061}" name="Proposed_QT_M_Agegrouped" dataDxfId="18"/>
+    <tableColumn id="51" xr3:uid="{4DA2C733-ABC7-49F3-87B2-5B3B3C0229C3}" name="Proposed_QT_M_Agegrouped_roundedup" dataDxfId="17">
       <calculatedColumnFormula>CEILING(Table1419[[#This Row],[Proposed_QT_M_Agegrouped]],"00:01:00")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="60" xr3:uid="{DDE641CD-619C-4667-8F18-FD3BF5239B65}" name="Proposed_QT_M_Agegrouped_roundedup_min" dataDxfId="18">
+    <tableColumn id="60" xr3:uid="{DDE641CD-619C-4667-8F18-FD3BF5239B65}" name="Proposed_QT_M_Agegrouped_roundedup_min" dataDxfId="16">
       <calculatedColumnFormula>Table1419[[#This Row],[Proposed_QT_M_Agegrouped_roundedup]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" xr3:uid="{2CA6AF2D-2E7B-4B32-B5FE-215E9CB0D627}" name="Time_diff_from_existing_M" dataDxfId="17">
+    <tableColumn id="59" xr3:uid="{2CA6AF2D-2E7B-4B32-B5FE-215E9CB0D627}" name="Time_diff_from_existing_M" dataDxfId="15">
       <calculatedColumnFormula>Table1419[[#This Row],[Proposed_QT_M_Agegrouped_roundedup_min]]-Table1419[[#This Row],[QT_Men_2020_min]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{6CF274B0-A43D-4A27-9535-2200F93DB923}" name="Percentage_diff_from_existing_M" dataDxfId="16">
+    <tableColumn id="53" xr3:uid="{6CF274B0-A43D-4A27-9535-2200F93DB923}" name="Percentage_diff_from_existing_M" dataDxfId="14">
       <calculatedColumnFormula>(Table1419[[#This Row],[Proposed_QT_M_Agegrouped_roundedup_min]]-Table1419[[#This Row],[QT_Men_2020_min]])/Table1419[[#This Row],[QT_Men_2020_min]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{D10EF195-9FDB-4A88-9885-012239C4A2F1}" name="Proposed_QT_W" dataDxfId="15">
+    <tableColumn id="47" xr3:uid="{D10EF195-9FDB-4A88-9885-012239C4A2F1}" name="Proposed_QT_W" dataDxfId="13">
       <calculatedColumnFormula>Table1419[[#This Row],[Age Best_Women]]/Table1419[[#This Row],[Proposed_uniform_AG%]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{5D881879-5CBE-42CE-B7A4-C0C3DEBCA8B8}" name="Proposed_QT_W_Agegrouped" dataDxfId="14"/>
-    <tableColumn id="54" xr3:uid="{087EBD6D-333C-4AAC-B820-F55F4319C83D}" name="Proposed_QT_W_Agegrouped_roundedup" dataDxfId="13">
+    <tableColumn id="48" xr3:uid="{5D881879-5CBE-42CE-B7A4-C0C3DEBCA8B8}" name="Proposed_QT_W_Agegrouped" dataDxfId="12"/>
+    <tableColumn id="54" xr3:uid="{087EBD6D-333C-4AAC-B820-F55F4319C83D}" name="Proposed_QT_W_Agegrouped_roundedup" dataDxfId="11">
       <calculatedColumnFormula>CEILING(Table1419[[#This Row],[Proposed_QT_W_Agegrouped]],"00:01:00")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="55" xr3:uid="{C0405CFF-5B8D-48A6-9942-EC627B32B8EB}" name="Proposed_QT_W_Agegrouped_roundedup_min" dataDxfId="12">
+    <tableColumn id="55" xr3:uid="{C0405CFF-5B8D-48A6-9942-EC627B32B8EB}" name="Proposed_QT_W_Agegrouped_roundedup_min" dataDxfId="10">
       <calculatedColumnFormula>Table1419[[#This Row],[Proposed_QT_W_Agegrouped_roundedup]]*1440</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="56" xr3:uid="{E3CE0CC5-644E-4F05-A948-C98FDE7AFE75}" name="Time_diff_from_existing_W" dataDxfId="11">
+    <tableColumn id="56" xr3:uid="{E3CE0CC5-644E-4F05-A948-C98FDE7AFE75}" name="Time_diff_from_existing_W" dataDxfId="9">
       <calculatedColumnFormula>Table1419[[#This Row],[Proposed_QT_W_Agegrouped_roundedup_min]]-Table1419[[#This Row],[Qualifying_Time_Women_2020_min]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="57" xr3:uid="{E4CAB471-549B-4C50-9F7A-CF2031C0188D}" name="Percentage_diff_from_existing_W" dataDxfId="10">
+    <tableColumn id="57" xr3:uid="{E4CAB471-549B-4C50-9F7A-CF2031C0188D}" name="Percentage_diff_from_existing_W" dataDxfId="8">
       <calculatedColumnFormula>(Table1419[[#This Row],[Proposed_QT_W_Agegrouped_roundedup_min]]-Table1419[[#This Row],[Qualifying_Time_Women_2020_min]])/Table1419[[#This Row],[Qualifying_Time_Women_2020_min]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="62" xr3:uid="{8516F639-258F-4CF0-AB9E-0947E3865301}" name="Age_group" dataDxfId="9"/>
-    <tableColumn id="63" xr3:uid="{2EE7365D-1460-4F57-911C-CCF7B165D513}" name="Proposed_AG%_men" dataDxfId="8">
+    <tableColumn id="62" xr3:uid="{8516F639-258F-4CF0-AB9E-0947E3865301}" name="Age_group" dataDxfId="7"/>
+    <tableColumn id="63" xr3:uid="{2EE7365D-1460-4F57-911C-CCF7B165D513}" name="Proposed_AG%_men" dataDxfId="6">
       <calculatedColumnFormula>Table1419[[#This Row],[Age Best_Men_20]]/Table1419[[#This Row],[Proposed_QT_M_Agegrouped_roundedup]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="64" xr3:uid="{81A585FD-471F-431D-B7AA-51F526127E2F}" name="Proposed_AG%_women" dataDxfId="7">
+    <tableColumn id="64" xr3:uid="{81A585FD-471F-431D-B7AA-51F526127E2F}" name="Proposed_AG%_women" dataDxfId="5">
       <calculatedColumnFormula>Table1419[[#This Row],[Age Best_Women]]/Table1419[[#This Row],[Proposed_QT_W_Agegrouped_roundedup]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3614,12 +3624,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7B6FC643-6BAD-413B-ACC8-58B69CA82DE1}" name="Table3" displayName="Table3" ref="A3:C13" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7B6FC643-6BAD-413B-ACC8-58B69CA82DE1}" name="Table3" displayName="Table3" ref="A3:C13" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A3:C13" xr:uid="{D43B58CF-5EBA-40DE-9C26-F84C383FB0B3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{73E2673F-5AA5-4A1A-86F2-4BB4A290341A}" name="Year" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{1E8D14A1-5293-487A-B957-F254C9A99695}" name="Men" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{7624C138-415A-4B01-8FA1-630F4CC2C6A8}" name="Women" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{73E2673F-5AA5-4A1A-86F2-4BB4A290341A}" name="Year" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{1E8D14A1-5293-487A-B957-F254C9A99695}" name="Men" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{7624C138-415A-4B01-8FA1-630F4CC2C6A8}" name="Women" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3939,14 +3949,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="17" t="s">
@@ -3972,10 +3982,10 @@
       <c r="A4" s="44">
         <v>18</v>
       </c>
-      <c r="B4" s="61">
+      <c r="B4" s="48">
         <v>0.67630000000000001</v>
       </c>
-      <c r="C4" s="61">
+      <c r="C4" s="48">
         <v>0.67630000000000001</v>
       </c>
       <c r="D4" s="45">
@@ -4138,16 +4148,16 @@
       <c r="A13" s="44">
         <v>54</v>
       </c>
-      <c r="B13" s="61">
+      <c r="B13" s="48">
         <v>0.68910000000000005</v>
       </c>
-      <c r="C13" s="61">
+      <c r="C13" s="48">
         <v>0.68910000000000005</v>
       </c>
-      <c r="D13" s="61">
+      <c r="D13" s="48">
         <v>0.67679999999999996</v>
       </c>
-      <c r="E13" s="61">
+      <c r="E13" s="48">
         <v>0.67679999999999996</v>
       </c>
       <c r="F13" s="46" t="s">
@@ -4158,16 +4168,16 @@
       <c r="A14" s="44">
         <v>55</v>
       </c>
-      <c r="B14" s="61">
+      <c r="B14" s="48">
         <v>0.66310000000000002</v>
       </c>
-      <c r="C14" s="61">
+      <c r="C14" s="48">
         <v>0.66310000000000002</v>
       </c>
-      <c r="D14" s="61">
+      <c r="D14" s="48">
         <v>0.65780000000000005</v>
       </c>
-      <c r="E14" s="61">
+      <c r="E14" s="48">
         <v>0.65780000000000005</v>
       </c>
       <c r="F14" s="46" t="s">
@@ -4361,12 +4371,12 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:C24">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="75" priority="4">
       <formula>$B4&lt;&gt;$C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:E24">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="74" priority="1">
       <formula>$D4&lt;&gt;$E4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4458,98 +4468,98 @@
       <c r="R2" s="6"/>
     </row>
     <row r="3" spans="1:86" x14ac:dyDescent="0.55000000000000004">
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="57" t="s">
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58">
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="61">
         <v>2020</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="W3" s="56" t="s">
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="61"/>
+      <c r="S3" s="61"/>
+      <c r="W3" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="57" t="s">
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="AC3" s="57"/>
-      <c r="AD3" s="57"/>
-      <c r="AE3" s="57"/>
-      <c r="AF3" s="57"/>
-      <c r="AG3" s="58">
+      <c r="AC3" s="60"/>
+      <c r="AD3" s="60"/>
+      <c r="AE3" s="60"/>
+      <c r="AF3" s="60"/>
+      <c r="AG3" s="61">
         <v>2020</v>
       </c>
-      <c r="AH3" s="58"/>
-      <c r="AI3" s="58"/>
-      <c r="AJ3" s="58"/>
-      <c r="AK3" s="58"/>
-      <c r="AL3" s="47" t="s">
+      <c r="AH3" s="61"/>
+      <c r="AI3" s="61"/>
+      <c r="AJ3" s="61"/>
+      <c r="AK3" s="61"/>
+      <c r="AL3" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="AM3" s="48"/>
-      <c r="AN3" s="48"/>
-      <c r="AO3" s="48"/>
-      <c r="AP3" s="48"/>
+      <c r="AM3" s="51"/>
+      <c r="AN3" s="51"/>
+      <c r="AO3" s="51"/>
+      <c r="AP3" s="51"/>
       <c r="AQ3" s="8"/>
     </row>
     <row r="4" spans="1:86" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="50" t="s">
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="50"/>
-      <c r="V4" s="50"/>
-      <c r="W4" s="50"/>
-      <c r="X4" s="50"/>
-      <c r="Y4" s="50"/>
-      <c r="Z4" s="50"/>
-      <c r="AA4" s="50"/>
-      <c r="AB4" s="50"/>
-      <c r="AC4" s="50"/>
-      <c r="AD4" s="50"/>
-      <c r="AE4" s="50"/>
-      <c r="AF4" s="50"/>
-      <c r="AG4" s="50"/>
-      <c r="AH4" s="50"/>
-      <c r="AI4" s="50"/>
-      <c r="AJ4" s="50"/>
-      <c r="AK4" s="50"/>
+      <c r="U4" s="53"/>
+      <c r="V4" s="53"/>
+      <c r="W4" s="53"/>
+      <c r="X4" s="53"/>
+      <c r="Y4" s="53"/>
+      <c r="Z4" s="53"/>
+      <c r="AA4" s="53"/>
+      <c r="AB4" s="53"/>
+      <c r="AC4" s="53"/>
+      <c r="AD4" s="53"/>
+      <c r="AE4" s="53"/>
+      <c r="AF4" s="53"/>
+      <c r="AG4" s="53"/>
+      <c r="AH4" s="53"/>
+      <c r="AI4" s="53"/>
+      <c r="AJ4" s="53"/>
+      <c r="AK4" s="53"/>
       <c r="AL4" s="9">
         <v>0.6</v>
       </c>
@@ -4565,22 +4575,22 @@
       <c r="AP4" s="11">
         <v>1</v>
       </c>
-      <c r="AR4" s="51" t="s">
+      <c r="AR4" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="AS4" s="52"/>
-      <c r="AT4" s="52"/>
-      <c r="AU4" s="52"/>
-      <c r="AV4" s="52"/>
-      <c r="AW4" s="53"/>
-      <c r="AX4" s="54" t="s">
+      <c r="AS4" s="55"/>
+      <c r="AT4" s="55"/>
+      <c r="AU4" s="55"/>
+      <c r="AV4" s="55"/>
+      <c r="AW4" s="56"/>
+      <c r="AX4" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="AY4" s="55"/>
-      <c r="AZ4" s="55"/>
-      <c r="BA4" s="55"/>
-      <c r="BB4" s="55"/>
-      <c r="BC4" s="55"/>
+      <c r="AY4" s="58"/>
+      <c r="AZ4" s="58"/>
+      <c r="BA4" s="58"/>
+      <c r="BB4" s="58"/>
+      <c r="BC4" s="58"/>
     </row>
     <row r="5" spans="1:86" s="17" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12" t="s">
@@ -20232,11 +20242,11 @@
         <v>2010</v>
       </c>
       <c r="B4" s="17">
-        <f>_xlfn.MAXIFS([4]!Table1[AgeOnRaceDay],[4]!Table1[Gender],"M")</f>
+        <f>_xlfn.MAXIFS([12]!Table1[AgeOnRaceDay],[12]!Table1[Gender],"M")</f>
         <v>81</v>
       </c>
       <c r="C4" s="17">
-        <f>_xlfn.MAXIFS([4]!Table1[AgeOnRaceDay],[4]!Table1[Gender],"F")</f>
+        <f>_xlfn.MAXIFS([12]!Table1[AgeOnRaceDay],[12]!Table1[Gender],"F")</f>
         <v>77</v>
       </c>
     </row>
@@ -20258,11 +20268,11 @@
         <v>2012</v>
       </c>
       <c r="B6" s="17">
-        <f>_xlfn.MAXIFS([5]!Table1[AgeOnRaceDay],[5]!Table1[Gender],"M")</f>
+        <f>_xlfn.MAXIFS([4]!Table1[AgeOnRaceDay],[4]!Table1[Gender],"M")</f>
         <v>83</v>
       </c>
       <c r="C6" s="17">
-        <f>_xlfn.MAXIFS([5]!Table1[AgeOnRaceDay],[5]!Table1[Gender],"F")</f>
+        <f>_xlfn.MAXIFS([4]!Table1[AgeOnRaceDay],[4]!Table1[Gender],"F")</f>
         <v>81</v>
       </c>
     </row>
@@ -20271,11 +20281,11 @@
         <v>2013</v>
       </c>
       <c r="B7" s="17">
-        <f>_xlfn.MAXIFS([6]!Table1[AgeOnRaceDay],[6]!Table1[Gender],"M")</f>
+        <f>_xlfn.MAXIFS([5]!Table1[AgeOnRaceDay],[5]!Table1[Gender],"M")</f>
         <v>80</v>
       </c>
       <c r="C7" s="17">
-        <f>_xlfn.MAXIFS([6]!Table1[AgeOnRaceDay],[6]!Table1[Gender],"F")</f>
+        <f>_xlfn.MAXIFS([5]!Table1[AgeOnRaceDay],[5]!Table1[Gender],"F")</f>
         <v>74</v>
       </c>
     </row>
@@ -20284,11 +20294,11 @@
         <v>2014</v>
       </c>
       <c r="B8" s="17">
-        <f>_xlfn.MAXIFS([7]!Table1[AgeOnRaceDay],[7]!Table1[Gender],"M")</f>
+        <f>_xlfn.MAXIFS([6]!Table1[AgeOnRaceDay],[6]!Table1[Gender],"M")</f>
         <v>81</v>
       </c>
       <c r="C8" s="17">
-        <f>_xlfn.MAXIFS([7]!Table1[AgeOnRaceDay],[7]!Table1[Gender],"F")</f>
+        <f>_xlfn.MAXIFS([6]!Table1[AgeOnRaceDay],[6]!Table1[Gender],"F")</f>
         <v>81</v>
       </c>
     </row>
@@ -20297,11 +20307,11 @@
         <v>2015</v>
       </c>
       <c r="B9" s="17">
-        <f>_xlfn.MAXIFS([8]!Table1[AgeOnRaceDay],[8]!Table1[Gender],"M")</f>
+        <f>_xlfn.MAXIFS([7]!Table1[AgeOnRaceDay],[7]!Table1[Gender],"M")</f>
         <v>82</v>
       </c>
       <c r="C9" s="17">
-        <f>_xlfn.MAXIFS([8]!Table1[AgeOnRaceDay],[8]!Table1[Gender],"F")</f>
+        <f>_xlfn.MAXIFS([7]!Table1[AgeOnRaceDay],[7]!Table1[Gender],"F")</f>
         <v>82</v>
       </c>
     </row>
@@ -20310,11 +20320,11 @@
         <v>2016</v>
       </c>
       <c r="B10" s="17">
-        <f>_xlfn.MAXIFS([9]!Table1[AgeOnRaceDay],[9]!Table1[Gender],"M")</f>
+        <f>_xlfn.MAXIFS([8]!Table1[AgeOnRaceDay],[8]!Table1[Gender],"M")</f>
         <v>83</v>
       </c>
       <c r="C10" s="17">
-        <f>_xlfn.MAXIFS([9]!Table1[AgeOnRaceDay],[9]!Table1[Gender],"F")</f>
+        <f>_xlfn.MAXIFS([8]!Table1[AgeOnRaceDay],[8]!Table1[Gender],"F")</f>
         <v>83</v>
       </c>
     </row>
@@ -20323,11 +20333,11 @@
         <v>2017</v>
       </c>
       <c r="B11" s="17">
-        <f>_xlfn.MAXIFS([10]!Table1[AgeOnRaceDay],[10]!Table1[Gender],"M")</f>
+        <f>_xlfn.MAXIFS([9]!Table1[AgeOnRaceDay],[9]!Table1[Gender],"M")</f>
         <v>83</v>
       </c>
       <c r="C11" s="17">
-        <f>_xlfn.MAXIFS([10]!Table1[AgeOnRaceDay],[10]!Table1[Gender],"F")</f>
+        <f>_xlfn.MAXIFS([9]!Table1[AgeOnRaceDay],[9]!Table1[Gender],"F")</f>
         <v>84</v>
       </c>
     </row>
@@ -20336,11 +20346,11 @@
         <v>2018</v>
       </c>
       <c r="B12" s="17">
-        <f>_xlfn.MAXIFS([11]!Table1[AgeOnRaceDay],[11]!Table1[Gender],"M")</f>
+        <f>_xlfn.MAXIFS([10]!Table1[AgeOnRaceDay],[10]!Table1[Gender],"M")</f>
         <v>82</v>
       </c>
       <c r="C12" s="17">
-        <f>_xlfn.MAXIFS([11]!Table1[AgeOnRaceDay],[11]!Table1[Gender],"F")</f>
+        <f>_xlfn.MAXIFS([10]!Table1[AgeOnRaceDay],[10]!Table1[Gender],"F")</f>
         <v>76</v>
       </c>
     </row>
@@ -20349,11 +20359,11 @@
         <v>2019</v>
       </c>
       <c r="B13" s="17">
-        <f>_xlfn.MAXIFS([12]!Table1[AgeOnRaceDay],[12]!Table1[Gender],"M")</f>
+        <f>_xlfn.MAXIFS([11]!Table1[AgeOnRaceDay],[11]!Table1[Gender],"M")</f>
         <v>83</v>
       </c>
       <c r="C13" s="17">
-        <f>_xlfn.MAXIFS([12]!Table1[AgeOnRaceDay],[12]!Table1[Gender],"F")</f>
+        <f>_xlfn.MAXIFS([11]!Table1[AgeOnRaceDay],[11]!Table1[Gender],"F")</f>
         <v>80</v>
       </c>
     </row>
@@ -20370,11 +20380,11 @@
   <dimension ref="A1:CX11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="CK2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="G18" sqref="G18"/>
       <selection pane="topRight" activeCell="G18" sqref="G18"/>
       <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
-      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomRight" activeCell="CM6" sqref="CM6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -21322,22 +21332,22 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:102" ht="130.80000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
     </row>
     <row r="8" spans="1:102" x14ac:dyDescent="0.4">
       <c r="J8" s="4"/>

</xml_diff>